<commit_message>
add functions for debuging and calibration.
</commit_message>
<xml_diff>
--- a/excel-data/robor22_r2.xlsx
+++ b/excel-data/robor22_r2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\2021\hexipitamaus\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7198F433-49B4-42B0-B197-548E909BAD49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3B35C6-8D5C-4AB4-A1FC-1F11A3721969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33132" yWindow="1080" windowWidth="26808" windowHeight="15024" activeTab="1" xr2:uid="{800E99C0-1BB9-4A49-B3EC-41CAC4F4573C}"/>
+    <workbookView xWindow="33132" yWindow="1080" windowWidth="26808" windowHeight="15024" activeTab="2" xr2:uid="{800E99C0-1BB9-4A49-B3EC-41CAC4F4573C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Degrees</t>
   </si>
@@ -155,6 +156,9 @@
   </si>
   <si>
     <t>motor angle 1</t>
+  </si>
+  <si>
+    <t>cal_pos</t>
   </si>
 </sst>
 </file>
@@ -1038,8 +1042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C891827A-283D-430E-B36B-9AA64D13A965}">
   <dimension ref="A2:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,15 +1130,15 @@
       </c>
       <c r="G6" s="4">
         <f>SUM((D6+D7-D5)/(2*B6*B7))</f>
-        <v>0.99741992703958693</v>
+        <v>0.47085494595234473</v>
       </c>
       <c r="H6">
         <f>SUM((D7+D5-D6)/(2*B7*B5))</f>
-        <v>0.99966271106098226</v>
+        <v>0.94770268340470609</v>
       </c>
       <c r="I6">
         <f>SUM((D5+D6-D7)/(2*B5*B6))</f>
-        <v>-0.99521914691427926</v>
+        <v>-0.1646689588087194</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -1143,26 +1147,26 @@
       </c>
       <c r="B7" s="23">
         <f>SUM(B10)</f>
-        <v>263.24893162176369</v>
+        <v>216.33538776631067</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>69300.000000000015</v>
+        <v>46801</v>
       </c>
       <c r="F7" t="s">
         <v>30</v>
       </c>
       <c r="G7">
         <f>ACOS(G6)</f>
-        <v>7.1849609423092708E-2</v>
+        <v>1.0805367040884015</v>
       </c>
       <c r="H7">
         <f>ACOS(H6)</f>
-        <v>2.5973367181071572E-2</v>
+        <v>0.32483724362158406</v>
       </c>
       <c r="I7">
         <f>ACOS(I6)</f>
-        <v>3.0437696769856286</v>
+        <v>1.7362187058798075</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -1172,15 +1176,15 @@
       </c>
       <c r="G8" s="18">
         <f>DEGREES(G7)</f>
-        <v>4.1166793796066017</v>
+        <v>61.910192753241731</v>
       </c>
       <c r="H8" s="6">
         <f>DEGREES(H7)</f>
-        <v>1.4881643192190053</v>
+        <v>18.611803088179688</v>
       </c>
       <c r="I8" s="19">
         <f>DEGREES(I7)</f>
-        <v>174.39515630117438</v>
+        <v>99.478004158578585</v>
       </c>
       <c r="J8">
         <f>SUM(G8:I8)</f>
@@ -1199,11 +1203,11 @@
       </c>
       <c r="B10" s="23">
         <f>SQRT(B11^2+B12^2)</f>
-        <v>263.24893162176369</v>
+        <v>216.33538776631067</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>69300.000000000015</v>
+        <v>46801</v>
       </c>
       <c r="G10" s="15" t="s">
         <v>27</v>
@@ -1229,15 +1233,15 @@
       </c>
       <c r="G11" s="4">
         <f>SUM((D11+D12-D10)/(2*B11*B12))</f>
-        <v>-2.58775253178901E-16</v>
+        <v>0</v>
       </c>
       <c r="H11">
         <f>SUM((D12+D10-D11)/(2*B12*B10))</f>
-        <v>0.89006055536002282</v>
+        <v>0.83205424510014436</v>
       </c>
       <c r="I11">
         <f>SUM((D10+D11-D12)/(2*B10*B11))</f>
-        <v>0.45584230583855201</v>
+        <v>0.55469427003605221</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -1246,26 +1250,26 @@
       </c>
       <c r="B12" s="20">
         <f>SUM(B26)</f>
-        <v>234.30749027719963</v>
+        <v>180.00277775634464</v>
       </c>
       <c r="D12" s="4">
         <f t="shared" si="0"/>
-        <v>54900</v>
+        <v>32401</v>
       </c>
       <c r="F12" t="s">
         <v>30</v>
       </c>
       <c r="G12">
         <f>ACOS(G11)</f>
-        <v>1.5707963267948968</v>
+        <v>1.5707963267948966</v>
       </c>
       <c r="H12">
         <f>ACOS(H11)</f>
-        <v>0.47331833171392623</v>
+        <v>0.58799548117149514</v>
       </c>
       <c r="I12">
         <f>ACOS(I11)</f>
-        <v>1.0974779950809701</v>
+        <v>0.98280084562340142</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1274,15 +1278,15 @@
       </c>
       <c r="G13" s="6">
         <f>DEGREES(G12)</f>
-        <v>90.000000000000014</v>
+        <v>90</v>
       </c>
       <c r="H13" s="6">
         <f>DEGREES(H12)</f>
-        <v>27.119142773381078</v>
+        <v>33.689659443890733</v>
       </c>
       <c r="I13" s="19">
         <f>DEGREES(I12)</f>
-        <v>62.880857226618907</v>
+        <v>56.310340556109267</v>
       </c>
       <c r="J13" s="7">
         <f>SUM(G13:I13)</f>
@@ -1325,7 +1329,7 @@
       </c>
       <c r="B19" s="17">
         <f>SUM(180-G28)</f>
-        <v>129.80557109226518</v>
+        <v>90.318306611451376</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
@@ -1334,7 +1338,7 @@
       </c>
       <c r="B20" s="17">
         <f>SUM(180 -(I13+G8))</f>
-        <v>113.00246339377449</v>
+        <v>61.779466690649002</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="25.8" x14ac:dyDescent="0.5">
@@ -1343,7 +1347,7 @@
       </c>
       <c r="B21" s="17">
         <f>SUM(360 - (I8 + 36 +90))</f>
-        <v>59.604843698825619</v>
+        <v>134.52199584142141</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1351,7 +1355,7 @@
         <v>38</v>
       </c>
       <c r="C23" s="14">
-        <v>150</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -1393,15 +1397,15 @@
       </c>
       <c r="B26" s="21">
         <f>SQRT(B25^2+B27^2)</f>
-        <v>234.30749027719963</v>
+        <v>180.00277775634464</v>
       </c>
       <c r="D26" s="4">
         <f t="shared" ref="D26:D27" si="1">SUM(B26^2)</f>
-        <v>54900</v>
+        <v>32401</v>
       </c>
       <c r="G26" s="4">
         <f>SUM((D26+D27-D25)/(2*B26*B27))</f>
-        <v>0.64018439966447982</v>
+        <v>5.5554698236580545E-3</v>
       </c>
       <c r="H26">
         <f>SUM((D27+D25-D26)/(2*B27*B25))</f>
@@ -1409,7 +1413,7 @@
       </c>
       <c r="I26">
         <f>SUM((D25+D26-D27)/(2*B25*B26))</f>
-        <v>0.76822127959737585</v>
+        <v>0.99998456825844984</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -1418,15 +1422,15 @@
       </c>
       <c r="B27">
         <f>SUM(C23)</f>
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
-        <v>22500</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <f>ACOS(G26)</f>
-        <v>0.87605805059819342</v>
+        <v>1.5652408283942039</v>
       </c>
       <c r="H27">
         <f>ACOS(H26)</f>
@@ -1434,13 +1438,13 @@
       </c>
       <c r="I27">
         <f>ACOS(I26)</f>
-        <v>0.69473827619670314</v>
+        <v>5.5554984007022412E-3</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="G28" s="19">
         <f>DEGREES(G27)</f>
-        <v>50.19442890773481</v>
+        <v>89.681693388548624</v>
       </c>
       <c r="H28" s="7">
         <f>DEGREES(H27)</f>
@@ -1448,11 +1452,136 @@
       </c>
       <c r="I28" s="7">
         <f>DEGREES(I27)</f>
-        <v>39.80557109226519</v>
+        <v>0.31830661145191708</v>
       </c>
       <c r="J28">
         <f>SUM(G28:I28)</f>
-        <v>180</v>
+        <v>180.00000000000057</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11B81173-4C77-4C96-B553-60A039B1EA67}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1">
+        <v>4.1611000000000002</v>
+      </c>
+      <c r="D1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="C2" s="7">
+        <f>SUM(B2*$C$1+$D$1)</f>
+        <v>183.22200000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C12" si="0">SUM(B3*$C$1+$D$1)</f>
+        <v>266.44400000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>349.66600000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>80</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>432.88800000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>90</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>474.49900000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>112</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>566.04320000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>130</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>640.94299999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>148</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>715.84280000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>166</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>790.74260000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>184</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>865.64240000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>202</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>940.54220000000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wip: prep for HH
</commit_message>
<xml_diff>
--- a/excel-data/robor22_r2.xlsx
+++ b/excel-data/robor22_r2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\2021\hexipitamaus\excel-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46517B9D-6B06-47CF-B448-8870BB02B61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5225D41-B7B9-4664-B68B-C752A28F34AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31620" yWindow="828" windowWidth="26808" windowHeight="15024" activeTab="2" xr2:uid="{800E99C0-1BB9-4A49-B3EC-41CAC4F4573C}"/>
+    <workbookView xWindow="31896" yWindow="756" windowWidth="26808" windowHeight="15024" activeTab="2" xr2:uid="{800E99C0-1BB9-4A49-B3EC-41CAC4F4573C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="75">
   <si>
     <t>Degrees</t>
   </si>
@@ -256,6 +256,12 @@
   </si>
   <si>
     <t>motor_3 angle</t>
+  </si>
+  <si>
+    <t>Negitive</t>
+  </si>
+  <si>
+    <t>https://www.mathsisfun.com/algebra/trig-solving-sss-triangles.html</t>
   </si>
 </sst>
 </file>
@@ -267,7 +273,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +347,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="8" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -409,6 +422,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -463,7 +482,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -494,11 +513,15 @@
     <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="9" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1597,10 +1620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B2209C-249A-4489-A47B-61E28798DE56}">
-  <dimension ref="A1:S28"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1635,8 +1658,8 @@
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2">
-        <v>220</v>
+      <c r="B2" s="29">
+        <v>150</v>
       </c>
       <c r="H2" t="s">
         <v>59</v>
@@ -1646,37 +1669,37 @@
       </c>
       <c r="J2" s="5">
         <f>SQRT(J4^2+J3^2)</f>
-        <v>221.19900542271884</v>
+        <v>151.75308893067054</v>
       </c>
       <c r="L2" t="s">
         <v>56</v>
       </c>
       <c r="N2">
         <f>SUM(N3:N4)</f>
-        <v>90</v>
+        <v>90.000000000000014</v>
       </c>
       <c r="P2" s="25">
         <f t="shared" ref="P2:P4" si="0">SUM(J2^2)</f>
-        <v>48929</v>
+        <v>23029.000000000004</v>
       </c>
       <c r="Q2">
         <f>SUM((P3+P4-P2)/(2*J3*J4))</f>
-        <v>0</v>
+        <v>-5.2724330537561056E-16</v>
       </c>
       <c r="R2">
         <f>ACOS(Q2)</f>
-        <v>1.5707963267948966</v>
+        <v>1.570796326794897</v>
       </c>
       <c r="S2">
         <f>DEGREES(R2)</f>
-        <v>90</v>
+        <v>90.000000000000028</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="29">
         <v>100</v>
       </c>
       <c r="H3" t="s">
@@ -1694,11 +1717,11 @@
       </c>
       <c r="M3">
         <f>ATAN2(J2,J3)</f>
-        <v>0.10360645484081366</v>
+        <v>0.15041721409454692</v>
       </c>
       <c r="N3">
         <f>DEGREES(M3)</f>
-        <v>5.9362125926913798</v>
+        <v>8.6182715337332585</v>
       </c>
       <c r="P3" s="25">
         <f t="shared" si="0"/>
@@ -1706,22 +1729,22 @@
       </c>
       <c r="Q3">
         <f>SUM((P4+P2-P3)/(2*J4*J2))</f>
-        <v>0.99457951711660042</v>
+        <v>0.98844775455298017</v>
       </c>
       <c r="R3">
         <f>ACOS(Q3)</f>
-        <v>0.10416704769945961</v>
+        <v>0.15214832643317466</v>
       </c>
       <c r="S3" s="5">
         <f>DEGREES(R3)</f>
-        <v>5.9683321975169674</v>
+        <v>8.7174569645996502</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="29">
         <v>23</v>
       </c>
       <c r="H4" t="s">
@@ -1732,34 +1755,34 @@
       </c>
       <c r="J4" s="5">
         <f>SUM(B2)</f>
-        <v>220</v>
+        <v>150</v>
       </c>
       <c r="L4" s="24" t="s">
         <v>8</v>
       </c>
       <c r="M4">
         <f>ATAN2(J3,J2)</f>
-        <v>1.467189871954083</v>
+        <v>1.4203791127003498</v>
       </c>
       <c r="N4">
         <f>DEGREES(M4)</f>
-        <v>84.063787407308624</v>
+        <v>81.38172846626675</v>
       </c>
       <c r="P4" s="25">
         <f t="shared" si="0"/>
-        <v>48400</v>
+        <v>22500</v>
       </c>
       <c r="Q4">
         <f>SUM((P2+P3-P4)/(2*J2*J3))</f>
-        <v>0.1039787676985537</v>
+        <v>0.15156198903145748</v>
       </c>
       <c r="R4">
         <f>ACOS(Q4)</f>
-        <v>1.4666292790954376</v>
+        <v>1.4186480003617212</v>
       </c>
       <c r="S4" s="5">
         <f>DEGREES(R4)</f>
-        <v>84.031667802483071</v>
+        <v>81.282543035400309</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -1791,7 +1814,7 @@
       </c>
       <c r="J7" s="5">
         <f>SQRT(J8^2+J9^2)</f>
-        <v>197.23082923316019</v>
+        <v>141.42135623730951</v>
       </c>
       <c r="L7" t="s">
         <v>56</v>
@@ -1804,7 +1827,7 @@
       </c>
       <c r="P7" s="25">
         <f>SUM(J7^2)</f>
-        <v>38900</v>
+        <v>20000</v>
       </c>
       <c r="Q7">
         <f>SUM((P8+P9-P7)/(2*J8*J9))</f>
@@ -1835,11 +1858,11 @@
       </c>
       <c r="M8">
         <f>ATAN2(J9,J8)</f>
-        <v>0.53172406725880561</v>
+        <v>0.78539816339744828</v>
       </c>
       <c r="N8">
         <f>DEGREES(M8)</f>
-        <v>30.46554491945988</v>
+        <v>45</v>
       </c>
       <c r="P8" s="25">
         <f t="shared" ref="P8:P9" si="1">SUM(J8^2)</f>
@@ -1847,15 +1870,15 @@
       </c>
       <c r="Q8">
         <f>SUM((P9+P7-P8)/(2*J9*J7))</f>
-        <v>0.86193421515776947</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="R8">
         <f>ACOS(Q8)</f>
-        <v>0.5317240672588055</v>
+        <v>0.78539816339744828</v>
       </c>
       <c r="S8" s="7">
         <f>DEGREES(R8)</f>
-        <v>30.465544919459877</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -1870,34 +1893,34 @@
       </c>
       <c r="J9" s="5">
         <f>SUM(J4-B6)</f>
-        <v>170</v>
+        <v>100</v>
       </c>
       <c r="L9" s="24" t="s">
         <v>8</v>
       </c>
       <c r="M9">
         <f>ATAN2(J8,J9)</f>
-        <v>1.0390722595360911</v>
+        <v>0.78539816339744828</v>
       </c>
       <c r="N9">
         <f>DEGREES(M9)</f>
-        <v>59.534455080540127</v>
+        <v>45</v>
       </c>
       <c r="P9" s="25">
         <f t="shared" si="1"/>
-        <v>28900</v>
+        <v>10000</v>
       </c>
       <c r="Q9">
         <f>SUM((P7+P8-P9)/(2*J7*J8))</f>
-        <v>0.5070201265633939</v>
+        <v>0.70710678118654746</v>
       </c>
       <c r="R9">
         <f>ACOS(Q9)</f>
-        <v>1.0390722595360908</v>
+        <v>0.78539816339744828</v>
       </c>
       <c r="S9" s="7">
         <f>DEGREES(R9)</f>
-        <v>59.534455080540113</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1936,15 +1959,15 @@
       </c>
       <c r="Q12">
         <f>SUM((P13+P14-P12)/(2*J13*J14))</f>
-        <v>0.22681962773588807</v>
+        <v>-0.66634041334223448</v>
       </c>
       <c r="R12">
         <f>ACOS(Q12)</f>
-        <v>1.3419853735947789</v>
+        <v>2.3000863538911185</v>
       </c>
       <c r="S12" s="6">
         <f>DEGREES(R12)</f>
-        <v>76.890098075267858</v>
+        <v>131.78524059359498</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1967,15 +1990,15 @@
       </c>
       <c r="Q13">
         <f>SUM((P14+P12-P13)/(2*J14*J12))</f>
-        <v>0.93960068295202859</v>
+        <v>0.96505578645633172</v>
       </c>
       <c r="R13">
         <f>ACOS(Q13)</f>
-        <v>0.34933455945514447</v>
+        <v>0.26514014375298234</v>
       </c>
       <c r="S13" s="6">
         <f>DEGREES(R13)</f>
-        <v>20.015395894841706</v>
+        <v>15.191411216537828</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1987,32 +2010,35 @@
       </c>
       <c r="J14" s="5">
         <f>SUM(J7)</f>
-        <v>197.23082923316019</v>
+        <v>141.42135623730951</v>
       </c>
       <c r="L14" t="s">
         <v>8</v>
       </c>
       <c r="P14" s="25">
         <f t="shared" si="2"/>
-        <v>38900</v>
+        <v>20000</v>
       </c>
       <c r="Q14">
         <f>SUM((P12+P13-P14)/(2*J12*J13))</f>
-        <v>0.12023203166658449</v>
+        <v>0.83844855639238536</v>
       </c>
       <c r="R14">
         <f>ACOS(Q14)</f>
-        <v>1.4502727205398698</v>
+        <v>0.57636615594569263</v>
       </c>
       <c r="S14" s="6">
         <f>DEGREES(R14)</f>
-        <v>83.094506029890439</v>
+        <v>33.023348189867228</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
       <c r="S15">
         <f>SUM(S12:S14)</f>
-        <v>180</v>
+        <v>180.00000000000003</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -2021,29 +2047,29 @@
       </c>
       <c r="B16" s="6">
         <f>SUM(S4)</f>
-        <v>84.031667802483071</v>
-      </c>
-      <c r="C16" s="28">
+        <v>81.282543035400309</v>
+      </c>
+      <c r="C16" s="27">
         <f>SUM(180-S4)</f>
-        <v>95.968332197516929</v>
+        <v>98.717456964599691</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="26">
         <f>SUM(180- (S9 +S12))</f>
-        <v>43.575446844192015</v>
+        <v>3.2147594064050224</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="27">
+      <c r="B18" s="26">
         <f>SUM(360 - S14 -126)</f>
-        <v>150.90549397010955</v>
+        <v>200.97665181013275</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
@@ -2093,21 +2119,33 @@
       <c r="B28">
         <v>123</v>
       </c>
-      <c r="I28" s="26" t="s">
+      <c r="I28" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
-      <c r="Q28" s="26"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28"/>
+      <c r="Q28" s="28"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="J30" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="K30" s="30"/>
+      <c r="L30" s="30"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="30"/>
+      <c r="O30" s="30"/>
+      <c r="P30" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I28:Q28"/>
+    <mergeCell ref="J30:P30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>